<commit_message>
Change UPDI buffer resistor to 0 Ohms. Internet recommendation of 1k didn't work. Not sure this is needed because of diode on UPDI 5V rail.
</commit_message>
<xml_diff>
--- a/hw/Overall Bill of Materials.xlsx
+++ b/hw/Overall Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Buetow\Projects\RGB LED Christmas Tree\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A149835A-0609-4BB8-ADE9-955A3BF50B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540D6387-00EA-4209-9A20-2CCE10B36D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9576" yWindow="5652" windowWidth="29220" windowHeight="18552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,24 +187,15 @@
     <t>5.1k Resistor</t>
   </si>
   <si>
-    <t>RES 1K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
     <t>Stackpole Electronics Inc</t>
   </si>
   <si>
-    <t>RMCF0603FT1K00</t>
-  </si>
-  <si>
     <t>Control: R1,R2</t>
   </si>
   <si>
     <t>Control: J3</t>
   </si>
   <si>
-    <t>1k Resistor</t>
-  </si>
-  <si>
     <t>10k Resistor</t>
   </si>
   <si>
@@ -311,6 +302,15 @@
   </si>
   <si>
     <t>Estimated filament for all base parts in kilograms</t>
+  </si>
+  <si>
+    <t>Jumper Resistor</t>
+  </si>
+  <si>
+    <t>RES 0 OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +786,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -821,7 +821,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -874,7 +874,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -918,7 +918,7 @@
         <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -962,7 +962,7 @@
         <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1006,7 +1006,7 @@
         <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1050,7 +1050,7 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G10">
         <f>4/80</f>
@@ -1086,10 +1086,10 @@
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1121,19 +1121,19 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1146,7 +1146,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="J12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1162,35 +1162,35 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" s="3">
-        <v>4.7999999999999996E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="I13" s="1">
         <f>Table1[[#This Row],[Unit Cost]]*Table1[[#This Row],[Unit QTY]]</f>
-        <v>4.7999999999999996E-3</v>
+        <v>4.3E-3</v>
       </c>
       <c r="J13">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1206,22 +1206,22 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1250,22 +1250,22 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
-      </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -1294,22 +1294,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
         <v>73</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" t="s">
-        <v>76</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1338,19 +1338,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
         <v>77</v>
       </c>
-      <c r="B17" t="s">
+      <c r="F17" t="s">
         <v>78</v>
-      </c>
-      <c r="C17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F17" t="s">
-        <v>81</v>
       </c>
       <c r="G17">
         <v>4</v>
@@ -1383,13 +1383,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1418,16 +1418,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1456,16 +1456,16 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
-        <v>93</v>
-      </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G20">
         <f>(61.7+18.4)/1000</f>
@@ -1495,16 +1495,16 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G21">
         <f>29/1000</f>
@@ -1665,7 +1665,7 @@
       <c r="H31"/>
       <c r="I31" s="6">
         <f>SUBTOTAL(109,Table1[Assy Cost])</f>
-        <v>8.9139999999999979</v>
+        <v>8.9134999999999991</v>
       </c>
       <c r="M31" s="5">
         <f>SUBTOTAL(109,Table1[Ext Cost])</f>

</xml_diff>